<commit_message>
Completed Exporting Data to a Text File
</commit_message>
<xml_diff>
--- a/17 - Importing and Exporting Data/Excel102Exercises.xlsx
+++ b/17 - Importing and Exporting Data/Excel102Exercises.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/16 - Excel Data Validation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sint-my.sharepoint.com/personal/james_cox_unifii_co_uk/Documents/Documents/Training/Udemy/Excel/MicrosoftExcelFromBeginnerToAdvanced/17 - Importing and Exporting Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="254" documentId="55C0F8F188DDD96CC547EB0156F2312C00657541" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1ED4E3E-9C70-4546-B7E1-8F1A2C144AFF}"/>
   <bookViews>
-    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="8" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16560" yWindow="-103" windowWidth="16663" windowHeight="8863" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2013" sheetId="1" r:id="rId1"/>
@@ -8779,7 +8779,7 @@
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
@@ -23796,7 +23796,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{793630A9-B3B0-4583-B3E0-4A1ECF629F1F}">
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>